<commit_message>
move "enter" button to right a bit
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/workflow.xlsx
+++ b/src/main/webapp/WEB-INF/book/workflow.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3398E37E-E4EB-014A-870D-092B719800EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'form list'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'submission list'!$C$6:$F$7</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
@@ -93,11 +94,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="36"/>
@@ -124,16 +120,19 @@
       <sz val="16"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -147,16 +146,19 @@
       <sz val="12"/>
       <color theme="1" tint="0.249977111117893"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF595959"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -168,16 +170,25 @@
       <sz val="12"/>
       <color rgb="FF404040"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -270,14 +281,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -285,56 +296,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -349,20 +360,20 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
@@ -640,7 +651,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
-    <tableStyle name="Table Style 2" pivot="0" count="5">
+    <tableStyle name="Table Style 2" pivot="0" count="5" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="14"/>
       <tableStyleElement type="headerRow" dxfId="13"/>
       <tableStyleElement type="firstRowStripe" dxfId="12"/>
@@ -658,6 +669,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -682,13 +696,13 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
+          <xdr:colOff>520700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>139700</xdr:colOff>
+          <xdr:colOff>469900</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -698,6 +712,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -730,9 +747,7 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
+                  <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Enter</a:t>
               </a:r>
@@ -771,6 +786,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -802,9 +820,7 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
+                  <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Leave</a:t>
               </a:r>
@@ -843,6 +859,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -874,9 +893,7 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
+                  <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Leave</a:t>
               </a:r>
@@ -892,23 +909,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table64" displayName="Table64" ref="C5:C12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table64" displayName="Table64" ref="C5:C12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="1">
-    <tableColumn id="1" name="Name" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C5:G7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="C5:G7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table5" displayName="Table5" ref="C5:G7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="C5:G7" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" name="Form" dataDxfId="3"/>
-    <tableColumn id="3" name="Owner" dataDxfId="2"/>
-    <tableColumn id="4" name="Status" dataDxfId="1"/>
-    <tableColumn id="5" name="Last Update" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Form" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Status" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Last Update" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1176,10 +1193,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="98" workbookViewId="0">
       <selection activeCell="E6" sqref="E6:G6"/>
     </sheetView>
   </sheetViews>
@@ -1365,7 +1382,7 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:G6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:G6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Employee, Supervisor"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1383,13 +1400,13 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>7</xdr:col>
-                    <xdr:colOff>190500</xdr:colOff>
+                    <xdr:colOff>520700</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>342900</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>139700</xdr:colOff>
+                    <xdr:colOff>469900</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1397,17 +1414,15 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1606,11 +1621,9 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <tableParts count="1">
     <tablePart r:id="rId4"/>
@@ -1619,7 +1632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1778,11 +1791,9 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <tableParts count="1">
     <tablePart r:id="rId4"/>

</xml_diff>